<commit_message>
update sizref peg2022  peg 2023
</commit_message>
<xml_diff>
--- a/data_in/translate_SIZRF.xlsx
+++ b/data_in/translate_SIZRF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\winfs-proj\data\proj\havgem\Mo-PROJEKTKATALOG\Uppdrag\HaV\Datavärdskapet_oceanografi_och_marinbiologi\2022\Städning\Translate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codes_shark\codes\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BCD8BD-AD2A-4C7F-970C-026F5346BFA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8600C-3BCB-4ACE-A2AE-2B3EE2EA97A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="3260" xr2:uid="{1A0B3E34-E74F-4EB7-997F-926D3A9788AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="136">
   <si>
     <t>PEG_BVOL2007</t>
   </si>
@@ -120,93 +120,33 @@
     <t>SMHI_BVOL2007</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2007 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2007 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2008</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2008 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2008 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2009</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2009 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2009 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2010</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2010 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2010 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2011</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2011 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2011 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2012</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2012 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2012 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2013</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2013 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2013 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2014</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2014 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2014 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2015</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2015 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2015 version</t>
-  </si>
-  <si>
     <t>SMHI_BVOL2016</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2016 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2016 version</t>
-  </si>
-  <si>
     <t>PHYTOWIN_U</t>
   </si>
   <si>
@@ -315,36 +255,6 @@
     <t>SMHI_BVOL2021</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2017 version</t>
-  </si>
-  <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2018 version</t>
-  </si>
-  <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2019 version</t>
-  </si>
-  <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2020 version</t>
-  </si>
-  <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2021 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2017 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2018 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2019 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2020 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2021 version</t>
-  </si>
-  <si>
     <t>SMHIBVOL_2017</t>
   </si>
   <si>
@@ -402,10 +312,127 @@
     <t>SMHI_BVOL2022</t>
   </si>
   <si>
-    <t>Biovolymer och storleksklasser av växtplankton i Skagerack och Kattegatt - 2022 version</t>
-  </si>
-  <si>
-    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerack and Kattegatt - 2022 version</t>
+    <t>PEG_BVOL2022</t>
+  </si>
+  <si>
+    <t>PEG_BVOL2023</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Östersjön - 2022 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Östersjön - 2023 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Baltic Sea - 2023 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Baltic Sea - 2022 version</t>
+  </si>
+  <si>
+    <t>SMHI_BVOL2023</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2007 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2008 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2009 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2010 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2011 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2012 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2013 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2014 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2015 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2016 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2017 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2018 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2019 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2020 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2021 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2022 version</t>
+  </si>
+  <si>
+    <t>Biovolumes and Size-classes of Phytoplankton in the Skagerrak and Kattegat - 2023 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2007 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2008 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2009 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2010 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2011 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2012 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2013 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2014 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2015 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2016 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2017 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2018 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2019 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2020 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2021 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2022 version</t>
+  </si>
+  <si>
+    <t>Biovolymer och storleksklasser av växtplankton i Skagerrak och Kattegatt - 2023 version</t>
   </si>
 </sst>
 </file>
@@ -801,58 +828,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23198DC7-7ECB-44AE-9516-21530A2BB8E3}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="83.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -864,19 +891,19 @@
         <v>2</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -888,19 +915,19 @@
         <v>5</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -912,19 +939,19 @@
         <v>8</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -936,19 +963,19 @@
         <v>11</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -960,19 +987,19 @@
         <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
@@ -984,19 +1011,19 @@
         <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1008,19 +1035,19 @@
         <v>20</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -1032,19 +1059,19 @@
         <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>24</v>
@@ -1056,19 +1083,19 @@
         <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>27</v>
@@ -1084,534 +1111,599 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="4"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="4"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>107</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="G27" s="5"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G29" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" t="s">
-        <v>110</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G30" s="5"/>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G31" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>126</v>
+      <c r="G32" t="s">
+        <v>80</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G33" s="5"/>
+      <c r="G33" t="s">
+        <v>81</v>
+      </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="5"/>
+        <v>117</v>
+      </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G35" s="6"/>
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G36" s="6"/>
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>